<commit_message>
"Create, Read, Update, and Delete" Lecture
</commit_message>
<xml_diff>
--- a/Logs/5th Week Logs.xlsx
+++ b/Logs/5th Week Logs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C2513F9-1073-4CD7-B50B-902744F578CC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA3A580-4764-46A8-A07C-98196952CA8C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -802,7 +802,7 @@
   <dimension ref="B2:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -910,7 +910,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="8">
-        <v>43521</v>
+        <v>43522</v>
       </c>
       <c r="D8" s="14">
         <v>0.75694444444444453</v>

</xml_diff>

<commit_message>
RazorPages Started + Broken project added
</commit_message>
<xml_diff>
--- a/Logs/5th Week Logs.xlsx
+++ b/Logs/5th Week Logs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EEE98B-A7CC-4541-86B6-C81423ECF322}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7340A3-D81F-4D93-866A-CEA7E895020D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -104,6 +104,18 @@
       </rPr>
       <t xml:space="preserve"> and relearning all from starting point</t>
     </r>
+  </si>
+  <si>
+    <t>Help</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Helping my friend to solve problems with VS + MVC </t>
+  </si>
+  <si>
+    <t>Practise</t>
+  </si>
+  <si>
+    <t>In class</t>
   </si>
 </sst>
 </file>
@@ -546,10 +558,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -835,7 +847,7 @@
   <dimension ref="B2:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1036,7 +1048,7 @@
       <c r="H11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="45" t="s">
+      <c r="I11" s="44" t="s">
         <v>17</v>
       </c>
       <c r="J11" s="4"/>
@@ -1070,27 +1082,57 @@
       <c r="J12" s="4"/>
       <c r="K12" s="41"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B13" s="38"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="44"/>
+    <row r="13" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B13" s="38">
+        <v>6</v>
+      </c>
+      <c r="C13" s="8">
+        <v>43528</v>
+      </c>
+      <c r="D13" s="14">
+        <v>0.79861111111111116</v>
+      </c>
+      <c r="E13" s="14">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="F13" s="4">
+        <v>10</v>
+      </c>
+      <c r="G13" s="12">
+        <v>120</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="45" t="s">
+        <v>19</v>
+      </c>
       <c r="J13" s="4"/>
       <c r="K13" s="41"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B14" s="38"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
+      <c r="B14" s="38">
+        <v>7</v>
+      </c>
+      <c r="C14" s="5">
+        <v>43525</v>
+      </c>
+      <c r="D14" s="14">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E14" s="14">
+        <v>0.41666666666666669</v>
+      </c>
       <c r="F14" s="4"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="43"/>
+      <c r="G14" s="12">
+        <v>120</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="43" t="s">
+        <v>21</v>
+      </c>
       <c r="J14" s="4"/>
       <c r="K14" s="41"/>
     </row>
@@ -1164,7 +1206,7 @@
       </c>
       <c r="G20" s="18">
         <f>SUM(G8:G19)</f>
-        <v>750</v>
+        <v>990</v>
       </c>
       <c r="H20" s="16"/>
       <c r="I20" s="16"/>

</xml_diff>